<commit_message>
add a rojmel pdf
</commit_message>
<xml_diff>
--- a/ROJMEL.xlsx
+++ b/ROJMEL.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\excle\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\excle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16E1A8D9-117C-4E29-9E14-776124F3BD1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BCA46CB-22F2-4D09-A3C7-F672A7A21390}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{113DD868-C34C-405C-98AB-405BB0E6F01D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="128">
   <si>
     <t>NO.</t>
   </si>
@@ -310,6 +310,114 @@
   </si>
   <si>
     <t>SUNIL (PETROL)</t>
+  </si>
+  <si>
+    <t>J. N. CO. RETURN</t>
+  </si>
+  <si>
+    <t>RAMKUMAR H. PANJVANI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DAINIKKUMAR A. DESAI </t>
+  </si>
+  <si>
+    <t>SHOP EXPENSES (BLANK PAGE)</t>
+  </si>
+  <si>
+    <t>SHUSILABEN R. PATEL</t>
+  </si>
+  <si>
+    <t>S.  K.  BANK (1717) CHECK</t>
+  </si>
+  <si>
+    <t>KALPANABEN V. PATEL</t>
+  </si>
+  <si>
+    <t>SAJANABEN PATEL</t>
+  </si>
+  <si>
+    <t>SHOP EXPENSES (MILK)</t>
+  </si>
+  <si>
+    <t>JAYESHBHAI H. THAKOR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VIRABHAI M. RABARI </t>
+  </si>
+  <si>
+    <t>HASAMUKHABHAI B. PATEL</t>
+  </si>
+  <si>
+    <t>PANNABEN D. DAVE</t>
+  </si>
+  <si>
+    <t>SIDHDHRAJ M. GADHAVI</t>
+  </si>
+  <si>
+    <t>RAVINDRASHINH A. CHAVADA</t>
+  </si>
+  <si>
+    <t>HIMESHKUMAR J. PARAMAR</t>
+  </si>
+  <si>
+    <t>JAYESHKUMAR L. PATEL</t>
+  </si>
+  <si>
+    <t>SHAILESHKUMAR K. PATEL</t>
+  </si>
+  <si>
+    <t>RIPERING (POLIS)</t>
+  </si>
+  <si>
+    <t>TARLIKABEN N. PATEL</t>
+  </si>
+  <si>
+    <t>KIRAPANSINH R. KUMPAVAT</t>
+  </si>
+  <si>
+    <t>DATTUBHAI</t>
+  </si>
+  <si>
+    <t>JAYANTIBHAI R. PARAMAR</t>
+  </si>
+  <si>
+    <t>SHOPE EXPENSES (JIMI</t>
+  </si>
+  <si>
+    <t>HASAMUKHBHAI S. PATEL</t>
+  </si>
+  <si>
+    <t>CHIRAGKUMAR P. CHAUDHARI</t>
+  </si>
+  <si>
+    <t>SHOPE EXPENSES (LEMINATION)</t>
+  </si>
+  <si>
+    <t>KAILASBEN N. LATA</t>
+  </si>
+  <si>
+    <t>HOME EXPENSES (JANTA DAIRY) KAMLESHBHAI</t>
+  </si>
+  <si>
+    <t>SHOPE EXPENSES (BREACKFAST)</t>
+  </si>
+  <si>
+    <t>ISHVERBHAI R. PATEL</t>
+  </si>
+  <si>
+    <t>PRUTHVISHINH S. PARMAR</t>
+  </si>
+  <si>
+    <t>MAKHKHBHOG (RENT RECIVE)</t>
+  </si>
+  <si>
+    <t>DEVENDRA K. PATEL</t>
+  </si>
+  <si>
+    <t>SHOP EXPENSES (TEA POWEDER)</t>
+  </si>
+  <si>
+    <t>ISHABEN M. RABARI</t>
   </si>
 </sst>
 </file>
@@ -319,7 +427,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -355,8 +463,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -366,6 +487,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -469,7 +596,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -510,12 +637,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -853,10 +985,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBD538BF-2A0D-4EFE-99B3-FCB30F79496D}">
-  <dimension ref="A1:E138"/>
+  <dimension ref="A1:E276"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A84" zoomScale="94" workbookViewId="0">
-      <selection activeCell="E141" sqref="E141"/>
+    <sheetView tabSelected="1" topLeftCell="A232" zoomScale="97" zoomScaleNormal="77" workbookViewId="0">
+      <selection activeCell="I242" sqref="I242"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -865,15 +997,15 @@
     <col min="2" max="2" width="15" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.5703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="35.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="12" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
       <c r="D1" s="13" t="s">
         <v>44</v>
       </c>
@@ -1449,7 +1581,7 @@
         <f>D41-D39</f>
         <v>-55</v>
       </c>
-      <c r="E42" s="7" t="s">
+      <c r="E42" s="21" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1490,11 +1622,11 @@
       <c r="E46" s="17"/>
     </row>
     <row r="47" spans="1:5" s="12" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A47" s="20" t="s">
+      <c r="A47" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="B47" s="21"/>
-      <c r="C47" s="21"/>
+      <c r="B47" s="24"/>
+      <c r="C47" s="24"/>
       <c r="D47" s="13" t="s">
         <v>44</v>
       </c>
@@ -1998,7 +2130,7 @@
         <f>D87-D85</f>
         <v>25</v>
       </c>
-      <c r="E88" s="19" t="s">
+      <c r="E88" s="22" t="s">
         <v>68</v>
       </c>
     </row>
@@ -2039,11 +2171,11 @@
       <c r="E92" s="7"/>
     </row>
     <row r="93" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A93" s="20" t="s">
+      <c r="A93" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="B93" s="21"/>
-      <c r="C93" s="21"/>
+      <c r="B93" s="24"/>
+      <c r="C93" s="24"/>
       <c r="D93" s="13" t="s">
         <v>44</v>
       </c>
@@ -2610,7 +2742,7 @@
         <f>D133-D131</f>
         <v>15</v>
       </c>
-      <c r="E134" s="19" t="s">
+      <c r="E134" s="20" t="s">
         <v>68</v>
       </c>
     </row>
@@ -2641,7 +2773,7 @@
       <c r="D137" s="8"/>
       <c r="E137" s="7"/>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A138" s="5">
         <v>44</v>
       </c>
@@ -2650,11 +2782,1616 @@
       <c r="D138" s="8"/>
       <c r="E138" s="7"/>
     </row>
+    <row r="139" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A139" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="B139" s="24"/>
+      <c r="C139" s="24"/>
+      <c r="D139" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="E139" s="14">
+        <f>DATE(2025,4,3)</f>
+        <v>45750</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A140" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B140" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C140" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D140" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E140" s="11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A141" s="5">
+        <v>1</v>
+      </c>
+      <c r="B141" s="8">
+        <f>D133</f>
+        <v>94050</v>
+      </c>
+      <c r="C141" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D141" s="8"/>
+      <c r="E141" s="7"/>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A142" s="5">
+        <v>2</v>
+      </c>
+      <c r="B142" s="8"/>
+      <c r="C142" s="7"/>
+      <c r="D142" s="8"/>
+      <c r="E142" s="7"/>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A143" s="5">
+        <v>3</v>
+      </c>
+      <c r="B143" s="8">
+        <v>48770</v>
+      </c>
+      <c r="C143" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D143" s="8">
+        <v>70</v>
+      </c>
+      <c r="E143" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A144" s="5">
+        <v>4</v>
+      </c>
+      <c r="B144" s="8">
+        <v>19500</v>
+      </c>
+      <c r="C144" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D144" s="8">
+        <v>730</v>
+      </c>
+      <c r="E144" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A145" s="5">
+        <v>5</v>
+      </c>
+      <c r="B145" s="8">
+        <v>100000</v>
+      </c>
+      <c r="C145" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="D145" s="8">
+        <v>210</v>
+      </c>
+      <c r="E145" s="7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A146" s="5">
+        <v>6</v>
+      </c>
+      <c r="B146" s="8">
+        <v>1405000</v>
+      </c>
+      <c r="C146" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="D146" s="8">
+        <v>1405000</v>
+      </c>
+      <c r="E146" s="7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A147" s="5">
+        <v>7</v>
+      </c>
+      <c r="B147" s="8">
+        <v>1400000</v>
+      </c>
+      <c r="C147" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="D147" s="8">
+        <v>1400000</v>
+      </c>
+      <c r="E147" s="7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A148" s="5">
+        <v>8</v>
+      </c>
+      <c r="B148" s="8">
+        <v>7200</v>
+      </c>
+      <c r="C148" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="D148" s="8">
+        <v>20</v>
+      </c>
+      <c r="E148" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A149" s="5">
+        <v>9</v>
+      </c>
+      <c r="B149" s="8">
+        <v>450</v>
+      </c>
+      <c r="C149" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="D149" s="8">
+        <v>70</v>
+      </c>
+      <c r="E149" s="7" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A150" s="5">
+        <v>10</v>
+      </c>
+      <c r="B150" s="8">
+        <v>5600</v>
+      </c>
+      <c r="C150" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="D150" s="8">
+        <v>50</v>
+      </c>
+      <c r="E150" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A151" s="5">
+        <v>11</v>
+      </c>
+      <c r="B151" s="8">
+        <v>10000</v>
+      </c>
+      <c r="C151" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="D151" s="8">
+        <v>3000</v>
+      </c>
+      <c r="E151" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A152" s="5">
+        <v>12</v>
+      </c>
+      <c r="B152" s="6">
+        <v>3200</v>
+      </c>
+      <c r="C152" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="D152" s="8">
+        <v>150</v>
+      </c>
+      <c r="E152" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A153" s="5">
+        <v>13</v>
+      </c>
+      <c r="B153" s="6">
+        <v>1200</v>
+      </c>
+      <c r="C153" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="D153" s="8">
+        <v>120</v>
+      </c>
+      <c r="E153" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A154" s="5">
+        <v>14</v>
+      </c>
+      <c r="B154" s="6">
+        <v>17800</v>
+      </c>
+      <c r="C154" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="D154" s="8">
+        <v>200</v>
+      </c>
+      <c r="E154" s="7" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A155" s="5">
+        <v>15</v>
+      </c>
+      <c r="B155" s="6">
+        <v>31000</v>
+      </c>
+      <c r="C155" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="D155" s="8">
+        <v>585</v>
+      </c>
+      <c r="E155" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A156" s="5">
+        <v>16</v>
+      </c>
+      <c r="B156" s="6">
+        <v>500</v>
+      </c>
+      <c r="C156" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="D156" s="8">
+        <v>30</v>
+      </c>
+      <c r="E156" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A157" s="5">
+        <v>17</v>
+      </c>
+      <c r="B157" s="6">
+        <v>3000</v>
+      </c>
+      <c r="C157" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="D157" s="8">
+        <v>3000</v>
+      </c>
+      <c r="E157" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A158" s="5">
+        <v>18</v>
+      </c>
+      <c r="B158" s="6">
+        <v>92500</v>
+      </c>
+      <c r="C158" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="D158" s="8">
+        <v>92500</v>
+      </c>
+      <c r="E158" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A159" s="5">
+        <v>19</v>
+      </c>
+      <c r="B159" s="6"/>
+      <c r="C159" s="7"/>
+      <c r="D159" s="8">
+        <v>10</v>
+      </c>
+      <c r="E159" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A160" s="5">
+        <v>20</v>
+      </c>
+      <c r="B160" s="6"/>
+      <c r="C160" s="7"/>
+      <c r="D160" s="8">
+        <v>100</v>
+      </c>
+      <c r="E160" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A161" s="5">
+        <v>21</v>
+      </c>
+      <c r="B161" s="6"/>
+      <c r="C161" s="7"/>
+      <c r="D161" s="8">
+        <v>5000</v>
+      </c>
+      <c r="E161" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A162" s="5">
+        <v>22</v>
+      </c>
+      <c r="B162" s="6"/>
+      <c r="C162" s="7"/>
+      <c r="D162" s="8">
+        <v>200</v>
+      </c>
+      <c r="E162" s="7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A163" s="5">
+        <v>23</v>
+      </c>
+      <c r="B163" s="6"/>
+      <c r="C163" s="7"/>
+      <c r="D163" s="8"/>
+      <c r="E163" s="7"/>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A164" s="5">
+        <v>24</v>
+      </c>
+      <c r="B164" s="6"/>
+      <c r="C164" s="7"/>
+      <c r="D164" s="8"/>
+      <c r="E164" s="7"/>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A165" s="5">
+        <v>25</v>
+      </c>
+      <c r="B165" s="6"/>
+      <c r="C165" s="7"/>
+      <c r="D165" s="8"/>
+      <c r="E165" s="7"/>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A166" s="5">
+        <v>26</v>
+      </c>
+      <c r="B166" s="6"/>
+      <c r="C166" s="7"/>
+      <c r="D166" s="8"/>
+      <c r="E166" s="7"/>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A167" s="5">
+        <v>27</v>
+      </c>
+      <c r="B167" s="6"/>
+      <c r="C167" s="7"/>
+      <c r="D167" s="8"/>
+      <c r="E167" s="7"/>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A168" s="5">
+        <v>28</v>
+      </c>
+      <c r="B168" s="6"/>
+      <c r="C168" s="7"/>
+      <c r="D168" s="8"/>
+      <c r="E168" s="7"/>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A169" s="5">
+        <v>29</v>
+      </c>
+      <c r="B169" s="6"/>
+      <c r="C169" s="7"/>
+      <c r="D169" s="8"/>
+      <c r="E169" s="7"/>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A170" s="5">
+        <v>30</v>
+      </c>
+      <c r="B170" s="6"/>
+      <c r="C170" s="7"/>
+      <c r="D170" s="8"/>
+      <c r="E170" s="7"/>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A171" s="5">
+        <v>31</v>
+      </c>
+      <c r="B171" s="6"/>
+      <c r="C171" s="7"/>
+      <c r="D171" s="8"/>
+      <c r="E171" s="7"/>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A172" s="5">
+        <v>32</v>
+      </c>
+      <c r="B172" s="6"/>
+      <c r="C172" s="7"/>
+      <c r="D172" s="8"/>
+      <c r="E172" s="7"/>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A173" s="5">
+        <v>33</v>
+      </c>
+      <c r="B173" s="6"/>
+      <c r="C173" s="7"/>
+      <c r="D173" s="8"/>
+      <c r="E173" s="7"/>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A174" s="5">
+        <v>34</v>
+      </c>
+      <c r="B174" s="6"/>
+      <c r="C174" s="7"/>
+      <c r="D174" s="8"/>
+      <c r="E174" s="7"/>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A175" s="5">
+        <v>35</v>
+      </c>
+      <c r="B175" s="6"/>
+      <c r="C175" s="7"/>
+      <c r="D175" s="8"/>
+      <c r="E175" s="7"/>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A176" s="5">
+        <v>36</v>
+      </c>
+      <c r="B176" s="6">
+        <f>SUM(B141:B174)</f>
+        <v>3239770</v>
+      </c>
+      <c r="C176" s="7"/>
+      <c r="D176" s="8">
+        <f>SUM(D143:D174)</f>
+        <v>2911045</v>
+      </c>
+      <c r="E176" s="7"/>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A177" s="5">
+        <v>37</v>
+      </c>
+      <c r="B177" s="6"/>
+      <c r="C177" s="7"/>
+      <c r="D177" s="8">
+        <f>B176-D176</f>
+        <v>328725</v>
+      </c>
+      <c r="E177" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A178" s="5">
+        <v>38</v>
+      </c>
+      <c r="B178" s="6"/>
+      <c r="C178" s="7"/>
+      <c r="D178" s="8"/>
+      <c r="E178" s="7"/>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A179" s="5">
+        <v>39</v>
+      </c>
+      <c r="B179" s="6"/>
+      <c r="C179" s="7"/>
+      <c r="D179" s="8">
+        <v>328720</v>
+      </c>
+      <c r="E179" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A180" s="5">
+        <v>40</v>
+      </c>
+      <c r="B180" s="6"/>
+      <c r="C180" s="7"/>
+      <c r="D180" s="8">
+        <f>D179-D177</f>
+        <v>-5</v>
+      </c>
+      <c r="E180" s="19" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A181" s="5">
+        <v>41</v>
+      </c>
+      <c r="B181" s="6"/>
+      <c r="C181" s="7"/>
+      <c r="D181" s="8"/>
+      <c r="E181" s="7"/>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A182" s="5">
+        <v>42</v>
+      </c>
+      <c r="B182" s="6"/>
+      <c r="C182" s="7"/>
+      <c r="D182" s="8"/>
+      <c r="E182" s="7"/>
+    </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A183" s="5">
+        <v>43</v>
+      </c>
+      <c r="B183" s="6"/>
+      <c r="C183" s="7"/>
+      <c r="D183" s="8"/>
+      <c r="E183" s="7"/>
+    </row>
+    <row r="184" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A184" s="5">
+        <v>44</v>
+      </c>
+      <c r="B184" s="6"/>
+      <c r="C184" s="7"/>
+      <c r="D184" s="8"/>
+      <c r="E184" s="7"/>
+    </row>
+    <row r="185" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A185" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="B185" s="24"/>
+      <c r="C185" s="24"/>
+      <c r="D185" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="E185" s="14">
+        <f>DATE(2025,4,4)</f>
+        <v>45751</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A186" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B186" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C186" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D186" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E186" s="11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A187" s="5">
+        <v>1</v>
+      </c>
+      <c r="B187" s="8">
+        <f>D179</f>
+        <v>328720</v>
+      </c>
+      <c r="C187" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D187" s="8"/>
+      <c r="E187" s="7"/>
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A188" s="5">
+        <v>2</v>
+      </c>
+      <c r="B188" s="8"/>
+      <c r="C188" s="7"/>
+      <c r="D188" s="8"/>
+      <c r="E188" s="7"/>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A189" s="5">
+        <v>3</v>
+      </c>
+      <c r="B189" s="8">
+        <v>5000</v>
+      </c>
+      <c r="C189" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="D189" s="8">
+        <v>432860</v>
+      </c>
+      <c r="E189" s="7" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A190" s="5">
+        <v>4</v>
+      </c>
+      <c r="B190" s="8">
+        <v>195000</v>
+      </c>
+      <c r="C190" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="D190" s="8">
+        <v>20000</v>
+      </c>
+      <c r="E190" s="7" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A191" s="5">
+        <v>5</v>
+      </c>
+      <c r="B191" s="8">
+        <v>1200</v>
+      </c>
+      <c r="C191" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="D191" s="8">
+        <v>20</v>
+      </c>
+      <c r="E191" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A192" s="5">
+        <v>6</v>
+      </c>
+      <c r="B192" s="8">
+        <v>471245</v>
+      </c>
+      <c r="C192" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="D192" s="8">
+        <v>471245</v>
+      </c>
+      <c r="E192" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A193" s="5">
+        <v>7</v>
+      </c>
+      <c r="B193" s="8">
+        <v>1300</v>
+      </c>
+      <c r="C193" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="D193" s="8">
+        <v>40</v>
+      </c>
+      <c r="E193" s="7" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A194" s="5">
+        <v>8</v>
+      </c>
+      <c r="B194" s="8">
+        <v>4000</v>
+      </c>
+      <c r="C194" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D194" s="8">
+        <v>20000</v>
+      </c>
+      <c r="E194" s="25" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A195" s="5">
+        <v>9</v>
+      </c>
+      <c r="B195" s="8">
+        <v>520</v>
+      </c>
+      <c r="C195" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D195" s="8">
+        <v>500</v>
+      </c>
+      <c r="E195" s="7" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A196" s="5">
+        <v>10</v>
+      </c>
+      <c r="B196" s="8">
+        <v>70000</v>
+      </c>
+      <c r="C196" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="D196" s="8">
+        <v>70000</v>
+      </c>
+      <c r="E196" s="7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A197" s="5">
+        <v>11</v>
+      </c>
+      <c r="B197" s="8">
+        <v>200000</v>
+      </c>
+      <c r="C197" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D197" s="8">
+        <v>950</v>
+      </c>
+      <c r="E197" s="7" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A198" s="5">
+        <v>12</v>
+      </c>
+      <c r="B198" s="6">
+        <v>47000</v>
+      </c>
+      <c r="C198" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="D198" s="8">
+        <v>60</v>
+      </c>
+      <c r="E198" s="7" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A199" s="5">
+        <v>13</v>
+      </c>
+      <c r="B199" s="6">
+        <v>2500</v>
+      </c>
+      <c r="C199" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="D199" s="8">
+        <v>2500</v>
+      </c>
+      <c r="E199" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A200" s="5">
+        <v>14</v>
+      </c>
+      <c r="B200" s="6"/>
+      <c r="C200" s="7"/>
+      <c r="D200" s="8">
+        <v>75</v>
+      </c>
+      <c r="E200" s="7" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A201" s="5">
+        <v>15</v>
+      </c>
+      <c r="B201" s="6"/>
+      <c r="C201" s="7"/>
+      <c r="D201" s="8">
+        <v>4000</v>
+      </c>
+      <c r="E201" s="7" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A202" s="5">
+        <v>16</v>
+      </c>
+      <c r="B202" s="6"/>
+      <c r="C202" s="7"/>
+      <c r="D202" s="8">
+        <v>100</v>
+      </c>
+      <c r="E202" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A203" s="5">
+        <v>17</v>
+      </c>
+      <c r="B203" s="6"/>
+      <c r="C203" s="7"/>
+      <c r="D203" s="8">
+        <v>2000</v>
+      </c>
+      <c r="E203" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A204" s="5">
+        <v>18</v>
+      </c>
+      <c r="B204" s="6"/>
+      <c r="C204" s="7"/>
+      <c r="D204" s="8"/>
+      <c r="E204" s="7"/>
+    </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A205" s="5">
+        <v>19</v>
+      </c>
+      <c r="B205" s="6"/>
+      <c r="C205" s="7"/>
+      <c r="D205" s="8"/>
+      <c r="E205" s="7"/>
+    </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A206" s="5">
+        <v>20</v>
+      </c>
+      <c r="B206" s="6"/>
+      <c r="C206" s="7"/>
+      <c r="D206" s="8"/>
+      <c r="E206" s="7"/>
+    </row>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A207" s="5">
+        <v>21</v>
+      </c>
+      <c r="B207" s="6"/>
+      <c r="C207" s="7"/>
+      <c r="D207" s="8"/>
+      <c r="E207" s="7"/>
+    </row>
+    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A208" s="5">
+        <v>22</v>
+      </c>
+      <c r="B208" s="6"/>
+      <c r="C208" s="7"/>
+      <c r="D208" s="8"/>
+      <c r="E208" s="7"/>
+    </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A209" s="5">
+        <v>23</v>
+      </c>
+      <c r="B209" s="6"/>
+      <c r="C209" s="7"/>
+      <c r="D209" s="8"/>
+      <c r="E209" s="7"/>
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A210" s="5">
+        <v>24</v>
+      </c>
+      <c r="B210" s="6"/>
+      <c r="C210" s="7"/>
+      <c r="D210" s="8"/>
+      <c r="E210" s="7"/>
+    </row>
+    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A211" s="5">
+        <v>25</v>
+      </c>
+      <c r="B211" s="6"/>
+      <c r="C211" s="7"/>
+      <c r="D211" s="8"/>
+      <c r="E211" s="7"/>
+    </row>
+    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A212" s="5">
+        <v>26</v>
+      </c>
+      <c r="B212" s="6"/>
+      <c r="C212" s="7"/>
+      <c r="D212" s="8"/>
+      <c r="E212" s="7"/>
+    </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A213" s="5">
+        <v>27</v>
+      </c>
+      <c r="B213" s="6"/>
+      <c r="C213" s="7"/>
+      <c r="D213" s="8"/>
+      <c r="E213" s="7"/>
+    </row>
+    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A214" s="5">
+        <v>28</v>
+      </c>
+      <c r="B214" s="6"/>
+      <c r="C214" s="7"/>
+      <c r="D214" s="8"/>
+      <c r="E214" s="7"/>
+    </row>
+    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A215" s="5">
+        <v>29</v>
+      </c>
+      <c r="B215" s="6"/>
+      <c r="C215" s="7"/>
+      <c r="D215" s="8"/>
+      <c r="E215" s="7"/>
+    </row>
+    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A216" s="5">
+        <v>30</v>
+      </c>
+      <c r="B216" s="6"/>
+      <c r="C216" s="7"/>
+      <c r="D216" s="8"/>
+      <c r="E216" s="7"/>
+    </row>
+    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A217" s="5">
+        <v>31</v>
+      </c>
+      <c r="B217" s="6"/>
+      <c r="C217" s="7"/>
+      <c r="D217" s="8"/>
+      <c r="E217" s="7"/>
+    </row>
+    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A218" s="5">
+        <v>32</v>
+      </c>
+      <c r="B218" s="6"/>
+      <c r="C218" s="7"/>
+      <c r="D218" s="8"/>
+      <c r="E218" s="7"/>
+    </row>
+    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A219" s="5">
+        <v>33</v>
+      </c>
+      <c r="B219" s="6"/>
+      <c r="C219" s="7"/>
+      <c r="D219" s="8"/>
+      <c r="E219" s="7"/>
+    </row>
+    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A220" s="5">
+        <v>34</v>
+      </c>
+      <c r="B220" s="6"/>
+      <c r="C220" s="7"/>
+      <c r="D220" s="8"/>
+      <c r="E220" s="7"/>
+    </row>
+    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A221" s="5">
+        <v>35</v>
+      </c>
+      <c r="B221" s="6"/>
+      <c r="C221" s="7"/>
+      <c r="D221" s="8"/>
+      <c r="E221" s="7"/>
+    </row>
+    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A222" s="5">
+        <v>36</v>
+      </c>
+      <c r="B222" s="6">
+        <f>SUM(B187:B220)</f>
+        <v>1326485</v>
+      </c>
+      <c r="C222" s="7"/>
+      <c r="D222" s="8">
+        <f>SUM(D189:D220)</f>
+        <v>1024350</v>
+      </c>
+      <c r="E222" s="7"/>
+    </row>
+    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A223" s="5">
+        <v>37</v>
+      </c>
+      <c r="B223" s="6"/>
+      <c r="C223" s="7"/>
+      <c r="D223" s="8">
+        <f>B222-D222</f>
+        <v>302135</v>
+      </c>
+      <c r="E223" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A224" s="5">
+        <v>38</v>
+      </c>
+      <c r="B224" s="6"/>
+      <c r="C224" s="7"/>
+      <c r="D224" s="8"/>
+      <c r="E224" s="7"/>
+    </row>
+    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A225" s="5">
+        <v>39</v>
+      </c>
+      <c r="B225" s="6"/>
+      <c r="C225" s="7"/>
+      <c r="D225" s="8">
+        <v>302175</v>
+      </c>
+      <c r="E225" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A226" s="5">
+        <v>40</v>
+      </c>
+      <c r="B226" s="6"/>
+      <c r="C226" s="7"/>
+      <c r="D226" s="8">
+        <f>D225-D223</f>
+        <v>40</v>
+      </c>
+      <c r="E226" s="20" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A227" s="5">
+        <v>41</v>
+      </c>
+      <c r="B227" s="6"/>
+      <c r="C227" s="7"/>
+      <c r="D227" s="8"/>
+      <c r="E227" s="7"/>
+    </row>
+    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A228" s="5">
+        <v>42</v>
+      </c>
+      <c r="B228" s="6"/>
+      <c r="C228" s="7"/>
+      <c r="D228" s="8"/>
+      <c r="E228" s="7"/>
+    </row>
+    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A229" s="5">
+        <v>43</v>
+      </c>
+      <c r="B229" s="6"/>
+      <c r="C229" s="7"/>
+      <c r="D229" s="8"/>
+      <c r="E229" s="7"/>
+    </row>
+    <row r="230" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A230" s="5">
+        <v>44</v>
+      </c>
+      <c r="B230" s="6"/>
+      <c r="C230" s="7"/>
+      <c r="D230" s="8"/>
+      <c r="E230" s="7"/>
+    </row>
+    <row r="231" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A231" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="B231" s="24"/>
+      <c r="C231" s="24"/>
+      <c r="D231" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="E231" s="14">
+        <f>DATE(2025,4,5)</f>
+        <v>45752</v>
+      </c>
+    </row>
+    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A232" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B232" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C232" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D232" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E232" s="11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A233" s="5">
+        <v>1</v>
+      </c>
+      <c r="B233" s="8">
+        <f>D225</f>
+        <v>302175</v>
+      </c>
+      <c r="C233" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D233" s="8"/>
+      <c r="E233" s="7"/>
+    </row>
+    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A234" s="5">
+        <v>2</v>
+      </c>
+      <c r="B234" s="8"/>
+      <c r="C234" s="7"/>
+      <c r="D234" s="8"/>
+      <c r="E234" s="7"/>
+    </row>
+    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A235" s="5">
+        <v>3</v>
+      </c>
+      <c r="B235" s="8"/>
+      <c r="C235" s="7"/>
+      <c r="D235" s="8"/>
+      <c r="E235" s="7"/>
+    </row>
+    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A236" s="5">
+        <v>4</v>
+      </c>
+      <c r="B236" s="8"/>
+      <c r="C236" s="7"/>
+      <c r="D236" s="8"/>
+      <c r="E236" s="7"/>
+    </row>
+    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A237" s="5">
+        <v>5</v>
+      </c>
+      <c r="B237" s="8"/>
+      <c r="C237" s="7"/>
+      <c r="D237" s="8"/>
+      <c r="E237" s="7"/>
+    </row>
+    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A238" s="5">
+        <v>6</v>
+      </c>
+      <c r="B238" s="8"/>
+      <c r="C238" s="7"/>
+      <c r="D238" s="8"/>
+      <c r="E238" s="7"/>
+    </row>
+    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A239" s="5">
+        <v>7</v>
+      </c>
+      <c r="B239" s="8"/>
+      <c r="C239" s="7"/>
+      <c r="D239" s="8"/>
+      <c r="E239" s="7"/>
+    </row>
+    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A240" s="5">
+        <v>8</v>
+      </c>
+      <c r="B240" s="8"/>
+      <c r="C240" s="7"/>
+      <c r="D240" s="8"/>
+      <c r="E240" s="26"/>
+    </row>
+    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A241" s="5">
+        <v>9</v>
+      </c>
+      <c r="B241" s="8"/>
+      <c r="C241" s="7"/>
+      <c r="D241" s="8"/>
+      <c r="E241" s="7"/>
+    </row>
+    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A242" s="5">
+        <v>10</v>
+      </c>
+      <c r="B242" s="8"/>
+      <c r="C242" s="7"/>
+      <c r="D242" s="8"/>
+      <c r="E242" s="7"/>
+    </row>
+    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A243" s="5">
+        <v>11</v>
+      </c>
+      <c r="B243" s="8"/>
+      <c r="C243" s="7"/>
+      <c r="D243" s="8"/>
+      <c r="E243" s="7"/>
+    </row>
+    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A244" s="5">
+        <v>12</v>
+      </c>
+      <c r="B244" s="6"/>
+      <c r="C244" s="7"/>
+      <c r="D244" s="8"/>
+      <c r="E244" s="7"/>
+    </row>
+    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A245" s="5">
+        <v>13</v>
+      </c>
+      <c r="B245" s="6"/>
+      <c r="C245" s="7"/>
+      <c r="D245" s="8"/>
+      <c r="E245" s="7"/>
+    </row>
+    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A246" s="5">
+        <v>14</v>
+      </c>
+      <c r="B246" s="6"/>
+      <c r="C246" s="7"/>
+      <c r="D246" s="8"/>
+      <c r="E246" s="7"/>
+    </row>
+    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A247" s="5">
+        <v>15</v>
+      </c>
+      <c r="B247" s="6"/>
+      <c r="C247" s="7"/>
+      <c r="D247" s="8"/>
+      <c r="E247" s="7"/>
+    </row>
+    <row r="248" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A248" s="5">
+        <v>16</v>
+      </c>
+      <c r="B248" s="6"/>
+      <c r="C248" s="7"/>
+      <c r="D248" s="8"/>
+      <c r="E248" s="7"/>
+    </row>
+    <row r="249" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A249" s="5">
+        <v>17</v>
+      </c>
+      <c r="B249" s="6"/>
+      <c r="C249" s="7"/>
+      <c r="D249" s="8"/>
+      <c r="E249" s="7"/>
+    </row>
+    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A250" s="5">
+        <v>18</v>
+      </c>
+      <c r="B250" s="6"/>
+      <c r="C250" s="7"/>
+      <c r="D250" s="8"/>
+      <c r="E250" s="7"/>
+    </row>
+    <row r="251" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A251" s="5">
+        <v>19</v>
+      </c>
+      <c r="B251" s="6"/>
+      <c r="C251" s="7"/>
+      <c r="D251" s="8"/>
+      <c r="E251" s="7"/>
+    </row>
+    <row r="252" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A252" s="5">
+        <v>20</v>
+      </c>
+      <c r="B252" s="6"/>
+      <c r="C252" s="7"/>
+      <c r="D252" s="8"/>
+      <c r="E252" s="7"/>
+    </row>
+    <row r="253" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A253" s="5">
+        <v>21</v>
+      </c>
+      <c r="B253" s="6"/>
+      <c r="C253" s="7"/>
+      <c r="D253" s="8"/>
+      <c r="E253" s="7"/>
+    </row>
+    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A254" s="5">
+        <v>22</v>
+      </c>
+      <c r="B254" s="6"/>
+      <c r="C254" s="7"/>
+      <c r="D254" s="8"/>
+      <c r="E254" s="7"/>
+    </row>
+    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A255" s="5">
+        <v>23</v>
+      </c>
+      <c r="B255" s="6"/>
+      <c r="C255" s="7"/>
+      <c r="D255" s="8"/>
+      <c r="E255" s="7"/>
+    </row>
+    <row r="256" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A256" s="5">
+        <v>24</v>
+      </c>
+      <c r="B256" s="6"/>
+      <c r="C256" s="7"/>
+      <c r="D256" s="8"/>
+      <c r="E256" s="7"/>
+    </row>
+    <row r="257" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A257" s="5">
+        <v>25</v>
+      </c>
+      <c r="B257" s="6"/>
+      <c r="C257" s="7"/>
+      <c r="D257" s="8"/>
+      <c r="E257" s="7"/>
+    </row>
+    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A258" s="5">
+        <v>26</v>
+      </c>
+      <c r="B258" s="6"/>
+      <c r="C258" s="7"/>
+      <c r="D258" s="8"/>
+      <c r="E258" s="7"/>
+    </row>
+    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A259" s="5">
+        <v>27</v>
+      </c>
+      <c r="B259" s="6"/>
+      <c r="C259" s="7"/>
+      <c r="D259" s="8"/>
+      <c r="E259" s="7"/>
+    </row>
+    <row r="260" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A260" s="5">
+        <v>28</v>
+      </c>
+      <c r="B260" s="6"/>
+      <c r="C260" s="7"/>
+      <c r="D260" s="8"/>
+      <c r="E260" s="7"/>
+    </row>
+    <row r="261" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A261" s="5">
+        <v>29</v>
+      </c>
+      <c r="B261" s="6"/>
+      <c r="C261" s="7"/>
+      <c r="D261" s="8"/>
+      <c r="E261" s="7"/>
+    </row>
+    <row r="262" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A262" s="5">
+        <v>30</v>
+      </c>
+      <c r="B262" s="6"/>
+      <c r="C262" s="7"/>
+      <c r="D262" s="8"/>
+      <c r="E262" s="7"/>
+    </row>
+    <row r="263" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A263" s="5">
+        <v>31</v>
+      </c>
+      <c r="B263" s="6"/>
+      <c r="C263" s="7"/>
+      <c r="D263" s="8"/>
+      <c r="E263" s="7"/>
+    </row>
+    <row r="264" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A264" s="5">
+        <v>32</v>
+      </c>
+      <c r="B264" s="6"/>
+      <c r="C264" s="7"/>
+      <c r="D264" s="8"/>
+      <c r="E264" s="7"/>
+    </row>
+    <row r="265" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A265" s="5">
+        <v>33</v>
+      </c>
+      <c r="B265" s="6"/>
+      <c r="C265" s="7"/>
+      <c r="D265" s="8"/>
+      <c r="E265" s="7"/>
+    </row>
+    <row r="266" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A266" s="5">
+        <v>34</v>
+      </c>
+      <c r="B266" s="6"/>
+      <c r="C266" s="7"/>
+      <c r="D266" s="8"/>
+      <c r="E266" s="7"/>
+    </row>
+    <row r="267" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A267" s="5">
+        <v>35</v>
+      </c>
+      <c r="B267" s="6"/>
+      <c r="C267" s="7"/>
+      <c r="D267" s="8"/>
+      <c r="E267" s="7"/>
+    </row>
+    <row r="268" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A268" s="5">
+        <v>36</v>
+      </c>
+      <c r="B268" s="6">
+        <f>SUM(B233:B266)</f>
+        <v>302175</v>
+      </c>
+      <c r="C268" s="7"/>
+      <c r="D268" s="8">
+        <f>SUM(D235:D266)</f>
+        <v>0</v>
+      </c>
+      <c r="E268" s="7"/>
+    </row>
+    <row r="269" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A269" s="5">
+        <v>37</v>
+      </c>
+      <c r="B269" s="6"/>
+      <c r="C269" s="7"/>
+      <c r="D269" s="8">
+        <f>B268-D268</f>
+        <v>302175</v>
+      </c>
+      <c r="E269" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="270" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A270" s="5">
+        <v>38</v>
+      </c>
+      <c r="B270" s="6"/>
+      <c r="C270" s="7"/>
+      <c r="D270" s="8"/>
+      <c r="E270" s="7"/>
+    </row>
+    <row r="271" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A271" s="5">
+        <v>39</v>
+      </c>
+      <c r="B271" s="6"/>
+      <c r="C271" s="7"/>
+      <c r="D271" s="8"/>
+      <c r="E271" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="272" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A272" s="5">
+        <v>40</v>
+      </c>
+      <c r="B272" s="6"/>
+      <c r="C272" s="7"/>
+      <c r="D272" s="8">
+        <f>D271-D269</f>
+        <v>-302175</v>
+      </c>
+      <c r="E272" s="20" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="273" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A273" s="5">
+        <v>41</v>
+      </c>
+      <c r="B273" s="6"/>
+      <c r="C273" s="7"/>
+      <c r="D273" s="8"/>
+      <c r="E273" s="7"/>
+    </row>
+    <row r="274" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A274" s="5">
+        <v>42</v>
+      </c>
+      <c r="B274" s="6"/>
+      <c r="C274" s="7"/>
+      <c r="D274" s="8"/>
+      <c r="E274" s="7"/>
+    </row>
+    <row r="275" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A275" s="5">
+        <v>43</v>
+      </c>
+      <c r="B275" s="6"/>
+      <c r="C275" s="7"/>
+      <c r="D275" s="8"/>
+      <c r="E275" s="7"/>
+    </row>
+    <row r="276" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A276" s="5">
+        <v>44</v>
+      </c>
+      <c r="B276" s="6"/>
+      <c r="C276" s="7"/>
+      <c r="D276" s="8"/>
+      <c r="E276" s="7"/>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="6">
+    <mergeCell ref="A231:C231"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A47:C47"/>
     <mergeCell ref="A93:C93"/>
+    <mergeCell ref="A139:C139"/>
+    <mergeCell ref="A185:C185"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>